<commit_message>
fucked it all up
</commit_message>
<xml_diff>
--- a/GodsUnchainedSourceOfTruth.xlsx
+++ b/GodsUnchainedSourceOfTruth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JIMBO\Desktop\XLTrail\xltrailTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JIMBO\Desktop\XLTrail - Copy\xltrailTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D6810B-4D8C-49F4-98C7-5D19D2A0E546}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFDB133-740B-4ED6-90AC-647362E05E4A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17680" xr2:uid="{770EED2D-E9A5-4A81-8429-54C42AC4F7E7}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,10 +459,10 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -476,13 +476,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -496,10 +496,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Revert "fucked it all up"
This reverts commit 25b10db1a91f548695c4e885642b74daa1ccde4e.
</commit_message>
<xml_diff>
--- a/GodsUnchainedSourceOfTruth.xlsx
+++ b/GodsUnchainedSourceOfTruth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JIMBO\Desktop\XLTrail - Copy\xltrailTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JIMBO\Desktop\XLTrail\xltrailTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFDB133-740B-4ED6-90AC-647362E05E4A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D6810B-4D8C-49F4-98C7-5D19D2A0E546}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17680" xr2:uid="{770EED2D-E9A5-4A81-8429-54C42AC4F7E7}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,10 +459,10 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -476,13 +476,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -496,10 +496,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>

</xml_diff>